<commit_message>
fix bug where the code was writing a.xlsx
</commit_message>
<xml_diff>
--- a/excel/a.xlsx
+++ b/excel/a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis\IdeaProjects\SynchExcel\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529A7ACC-B73B-411C-81AB-343031134CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A5B13C-6EBA-4287-B42D-4155834B615B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1470" windowWidth="21600" windowHeight="12240" tabRatio="235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="3360" windowWidth="21600" windowHeight="12240" tabRatio="235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" ΦΥΛΛΟ 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">' ΦΥΛΛΟ 1'!$A$12:$T$687</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">' ΦΥΛΛΟ 1'!$A$12:$T$689</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$J$624</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'για εκτυπωση'!$A$4:$K$240</definedName>
     <definedName name="CATEGORIES">LIST!$C$8:$C$41</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3944" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1030">
   <si>
     <t>ΑΠΟΘΗΚΗ ΚΑΤΩ</t>
   </si>
@@ -3432,6 +3432,18 @@
   </si>
   <si>
     <t>ΤΕΛΕΥΤΑΙΑ ΤΙΜΗ ΑΓΟΡΑΣ</t>
+  </si>
+  <si>
+    <t>5998711723491</t>
+  </si>
+  <si>
+    <t>ΣOKOΛ. MILKA KAPAMEΛA 100GRX15</t>
+  </si>
+  <si>
+    <t>8711800114157</t>
+  </si>
+  <si>
+    <t>PRONTO KPEMA 12X250ML</t>
   </si>
 </sst>
 </file>
@@ -4929,35 +4941,35 @@
   <dimension ref="A1:T1475"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="12" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="R22" sqref="R22"/>
+      <selection pane="bottomRight" activeCell="B440" sqref="B440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="249" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="280" customWidth="1"/>
-    <col min="4" max="4" width="58" style="150" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" style="241" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="18" style="8" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="50" style="8" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="39.85546875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="8" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="24" style="125" customWidth="1"/>
-    <col min="19" max="19" width="69.7109375" style="8" customWidth="1"/>
-    <col min="20" max="20" width="26.140625" style="123" customWidth="1"/>
-    <col min="21" max="16384" width="14.42578125" style="8"/>
+    <col min="1" max="1" width="16.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.5703125" style="249" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.5703125" style="280" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58" style="150" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="48.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="53.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.42578125" style="241" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18" style="8" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="50" style="8" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="24" style="125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="69.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="26.140625" style="123" customWidth="1" collapsed="1"/>
+    <col min="21" max="16384" width="14.42578125" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" x14ac:dyDescent="0.4">
@@ -24811,7 +24823,9 @@
     <row r="440" spans="1:20" s="107" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A440" s="10"/>
       <c r="B440" s="10"/>
-      <c r="C440" s="10"/>
+      <c r="C440" s="10">
+        <v>0.68</v>
+      </c>
       <c r="D440" s="152">
         <v>1160037900</v>
       </c>
@@ -35348,7 +35362,9 @@
     <row r="674" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A674" s="10"/>
       <c r="B674" s="10"/>
-      <c r="C674" s="10"/>
+      <c r="C674" s="10">
+        <v>0.64</v>
+      </c>
       <c r="D674" s="152" t="s">
         <v>886</v>
       </c>
@@ -36008,74 +36024,93 @@
       <c r="T687" s="179"/>
     </row>
     <row r="688" spans="1:20" ht="27" x14ac:dyDescent="0.35">
-      <c r="F688" s="1"/>
-      <c r="O688" s="1"/>
-    </row>
-    <row r="689" spans="6:15" ht="27" x14ac:dyDescent="0.35">
-      <c r="F689" s="1"/>
-      <c r="J689" s="4"/>
-      <c r="O689" s="1"/>
-    </row>
-    <row r="690" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+      <c r="C688">
+        <v>0.70479999999999998</v>
+      </c>
+      <c r="E688" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F688" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G688">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="689" spans="3:15" ht="27" x14ac:dyDescent="0.35">
+      <c r="C689">
+        <v>3.1</v>
+      </c>
+      <c r="E689" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F689" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G689">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="690" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F690" s="1"/>
       <c r="J690" s="4"/>
       <c r="O690" s="1"/>
     </row>
-    <row r="691" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="691" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F691" s="1"/>
       <c r="J691" s="4"/>
       <c r="O691" s="1"/>
     </row>
-    <row r="692" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="692" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F692" s="1"/>
       <c r="J692" s="6"/>
       <c r="O692" s="1"/>
     </row>
-    <row r="693" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="693" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F693" s="1"/>
       <c r="O693" s="1"/>
     </row>
-    <row r="694" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="694" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F694" s="1"/>
       <c r="O694" s="1"/>
     </row>
-    <row r="695" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="695" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F695" s="1"/>
       <c r="O695" s="1"/>
     </row>
-    <row r="696" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="696" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F696" s="1"/>
       <c r="O696" s="1"/>
     </row>
-    <row r="697" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="697" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F697" s="1"/>
       <c r="O697" s="1"/>
     </row>
-    <row r="698" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="698" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F698" s="1"/>
       <c r="O698" s="1"/>
     </row>
-    <row r="699" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="699" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F699" s="1"/>
       <c r="O699" s="1"/>
     </row>
-    <row r="700" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="700" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F700" s="1"/>
       <c r="O700" s="1"/>
     </row>
-    <row r="701" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="701" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F701" s="1"/>
       <c r="O701" s="1"/>
     </row>
-    <row r="702" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="702" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F702" s="1"/>
       <c r="O702" s="1"/>
     </row>
-    <row r="703" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="703" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F703" s="1"/>
       <c r="O703" s="1"/>
     </row>
-    <row r="704" spans="6:15" ht="27" x14ac:dyDescent="0.35">
+    <row r="704" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F704" s="1"/>
       <c r="O704" s="1"/>
     </row>
@@ -39164,6 +39199,7 @@
       <c r="O1475" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A12:T689" xr:uid="{AEB22C3B-2387-42D1-90F7-9A70021B8E2D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E13:S632">
     <sortCondition ref="O13:O632"/>
     <sortCondition ref="F13:F632"/>
@@ -39226,18 +39262,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="251" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="237" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" style="251" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="251" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="251" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="251" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="251" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="251" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" style="251" customWidth="1"/>
-    <col min="10" max="10" width="69.7109375" style="251" customWidth="1"/>
-    <col min="11" max="11" width="46.140625" style="251" customWidth="1"/>
-    <col min="12" max="16384" width="14.42578125" style="251"/>
+    <col min="1" max="1" width="16.85546875" style="251" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.5703125" style="237" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="87.85546875" style="251" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" style="251" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.85546875" style="251" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="39.85546875" style="251" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" style="251" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.28515625" style="251" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.85546875" style="251" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.7109375" style="251" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.140625" style="251" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="14.42578125" style="251" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.4">
@@ -48512,7 +48548,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
@@ -48909,14 +48945,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47" defaultRowHeight="110.1" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="47" style="185"/>
-    <col min="2" max="2" width="101.28515625" style="148" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="204" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" style="204" customWidth="1"/>
-    <col min="5" max="8" width="47" style="185"/>
-    <col min="9" max="9" width="62.7109375" style="149" customWidth="1"/>
-    <col min="10" max="10" width="66.7109375" style="185" customWidth="1"/>
-    <col min="11" max="16384" width="47" style="185"/>
+    <col min="1" max="1" width="47" style="185" collapsed="1"/>
+    <col min="2" max="2" width="101.28515625" style="148" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" style="204" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.85546875" style="204" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="47" style="185" collapsed="1"/>
+    <col min="9" max="9" width="62.7109375" style="149" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="66.7109375" style="185" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="47" style="185" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="213" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
changed configuration and updated excel
</commit_message>
<xml_diff>
--- a/excel/a.xlsx
+++ b/excel/a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis\IdeaProjects\SynchExcel\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A5B13C-6EBA-4287-B42D-4155834B615B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6634F4-8ECA-4F65-B1E9-DF14E14F6F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="3360" windowWidth="21600" windowHeight="12240" tabRatio="235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="1065" windowWidth="21600" windowHeight="12240" tabRatio="235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" ΦΥΛΛΟ 1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3944" uniqueCount="1026">
   <si>
     <t>ΑΠΟΘΗΚΗ ΚΑΤΩ</t>
   </si>
@@ -3432,18 +3432,6 @@
   </si>
   <si>
     <t>ΤΕΛΕΥΤΑΙΑ ΤΙΜΗ ΑΓΟΡΑΣ</t>
-  </si>
-  <si>
-    <t>5998711723491</t>
-  </si>
-  <si>
-    <t>ΣOKOΛ. MILKA KAPAMEΛA 100GRX15</t>
-  </si>
-  <si>
-    <t>8711800114157</t>
-  </si>
-  <si>
-    <t>PRONTO KPEMA 12X250ML</t>
   </si>
 </sst>
 </file>
@@ -4941,10 +4929,10 @@
   <dimension ref="A1:T1475"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="12" topLeftCell="B687" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B440" sqref="B440"/>
+      <selection pane="bottomRight" activeCell="C688" sqref="C688:G689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -36024,32 +36012,16 @@
       <c r="T687" s="179"/>
     </row>
     <row r="688" spans="1:20" ht="27" x14ac:dyDescent="0.35">
-      <c r="C688">
-        <v>0.70479999999999998</v>
-      </c>
-      <c r="E688" t="s">
-        <v>1026</v>
-      </c>
-      <c r="F688" t="s">
-        <v>1027</v>
-      </c>
-      <c r="G688">
-        <v>4</v>
-      </c>
+      <c r="C688"/>
+      <c r="E688"/>
+      <c r="F688"/>
+      <c r="G688"/>
     </row>
     <row r="689" spans="3:15" ht="27" x14ac:dyDescent="0.35">
-      <c r="C689">
-        <v>3.1</v>
-      </c>
-      <c r="E689" t="s">
-        <v>1028</v>
-      </c>
-      <c r="F689" t="s">
-        <v>1029</v>
-      </c>
-      <c r="G689">
-        <v>2</v>
-      </c>
+      <c r="C689"/>
+      <c r="E689"/>
+      <c r="F689"/>
+      <c r="G689"/>
     </row>
     <row r="690" spans="3:15" ht="27" x14ac:dyDescent="0.35">
       <c r="F690" s="1"/>

</xml_diff>